<commit_message>
[excel] edit cell data-type
</commit_message>
<xml_diff>
--- a/result_5-iteration.xlsx
+++ b/result_5-iteration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\UNAIR\SKRIPSI\skripsi-py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3700AA47-BCD4-4876-BBBD-2629F6116B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920406CD-825D-4891-ACD0-C857774F0772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9948" yWindow="612" windowWidth="13044" windowHeight="10464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4584" yWindow="1248" windowWidth="13044" windowHeight="10464" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$H$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -134,15 +145,14 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,12 +463,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9" style="6"/>
+    <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -484,7 +494,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -510,7 +520,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -536,7 +546,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5">
+      <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
@@ -562,7 +572,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5">
+      <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -588,7 +598,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5">
+      <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -614,7 +624,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5">
+      <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -640,7 +650,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5">
+      <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -666,7 +676,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5">
+      <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
@@ -692,7 +702,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5">
+      <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
@@ -718,7 +728,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
@@ -744,7 +754,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5">
+      <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" t="s">
@@ -770,7 +780,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>4</v>
       </c>
       <c r="B13" t="s">
@@ -796,7 +806,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
@@ -822,7 +832,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>4</v>
       </c>
       <c r="B15" t="s">
@@ -848,7 +858,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5">
+      <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" t="s">
@@ -874,7 +884,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
@@ -900,7 +910,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="5">
+      <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" t="s">
@@ -926,7 +936,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>4</v>
       </c>
       <c r="B19" t="s">
@@ -952,7 +962,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="5">
+      <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
@@ -978,7 +988,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="5">
+      <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
@@ -1004,7 +1014,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="5">
+      <c r="A22">
         <v>4</v>
       </c>
       <c r="B22" t="s">
@@ -1030,7 +1040,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="5">
+      <c r="A23">
         <v>4</v>
       </c>
       <c r="B23" t="s">
@@ -1056,7 +1066,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="5">
+      <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" t="s">
@@ -1082,7 +1092,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="5">
+      <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
@@ -1108,7 +1118,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="5">
+      <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
@@ -1134,7 +1144,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="5">
+      <c r="A27">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -1160,7 +1170,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="5">
+      <c r="A28">
         <v>5</v>
       </c>
       <c r="B28" t="s">
@@ -1186,7 +1196,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="5">
+      <c r="A29">
         <v>5</v>
       </c>
       <c r="B29" t="s">
@@ -1212,7 +1222,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="5">
+      <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
@@ -1238,7 +1248,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="5">
+      <c r="A31">
         <v>5</v>
       </c>
       <c r="B31" t="s">
@@ -1264,7 +1274,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="5">
+      <c r="A32">
         <v>5</v>
       </c>
       <c r="B32" t="s">
@@ -1290,7 +1300,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="5">
+      <c r="A33">
         <v>5</v>
       </c>
       <c r="B33" t="s">
@@ -1316,7 +1326,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="5">
+      <c r="A34">
         <v>5</v>
       </c>
       <c r="B34" t="s">
@@ -1342,7 +1352,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="5">
+      <c r="A35">
         <v>5</v>
       </c>
       <c r="B35" t="s">
@@ -1368,7 +1378,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="5">
+      <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
@@ -1394,7 +1404,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="5">
+      <c r="A37">
         <v>5</v>
       </c>
       <c r="B37" t="s">
@@ -1420,7 +1430,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="5">
+      <c r="A38">
         <v>5</v>
       </c>
       <c r="B38" t="s">
@@ -1446,7 +1456,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="5">
+      <c r="A39">
         <v>5</v>
       </c>
       <c r="B39" t="s">
@@ -1472,7 +1482,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="5">
+      <c r="A40">
         <v>5</v>
       </c>
       <c r="B40" t="s">
@@ -1498,7 +1508,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="5">
+      <c r="A41">
         <v>5</v>
       </c>
       <c r="B41" t="s">
@@ -1524,7 +1534,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="5">
+      <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" t="s">
@@ -1550,7 +1560,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="5">
+      <c r="A43">
         <v>5</v>
       </c>
       <c r="B43" t="s">
@@ -1576,7 +1586,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="5">
+      <c r="A44">
         <v>5</v>
       </c>
       <c r="B44" t="s">
@@ -1602,7 +1612,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="5">
+      <c r="A45">
         <v>5</v>
       </c>
       <c r="B45" t="s">
@@ -1628,7 +1638,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="5">
+      <c r="A46">
         <v>5</v>
       </c>
       <c r="B46" t="s">
@@ -1654,7 +1664,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="5">
+      <c r="A47">
         <v>5</v>
       </c>
       <c r="B47" t="s">
@@ -1680,7 +1690,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="5">
+      <c r="A48">
         <v>5</v>
       </c>
       <c r="B48" t="s">
@@ -1706,7 +1716,7 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="5">
+      <c r="A49">
         <v>5</v>
       </c>
       <c r="B49" t="s">
@@ -1732,7 +1742,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="5">
+      <c r="A50">
         <v>5</v>
       </c>
       <c r="B50" t="s">
@@ -1758,7 +1768,7 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="5">
+      <c r="A51">
         <v>5</v>
       </c>
       <c r="B51" t="s">
@@ -1784,7 +1794,7 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="8">
+      <c r="A52" s="6">
         <v>10</v>
       </c>
       <c r="B52" t="s">
@@ -1810,7 +1820,7 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="5">
+      <c r="A53">
         <v>10</v>
       </c>
       <c r="B53" t="s">
@@ -1836,7 +1846,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="5">
+      <c r="A54">
         <v>10</v>
       </c>
       <c r="B54" t="s">
@@ -1862,7 +1872,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="5">
+      <c r="A55">
         <v>10</v>
       </c>
       <c r="B55" t="s">
@@ -1888,7 +1898,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="5">
+      <c r="A56">
         <v>10</v>
       </c>
       <c r="B56" t="s">
@@ -1914,7 +1924,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="5">
+      <c r="A57">
         <v>10</v>
       </c>
       <c r="B57" t="s">
@@ -1940,7 +1950,7 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="5">
+      <c r="A58">
         <v>10</v>
       </c>
       <c r="B58" t="s">
@@ -1966,7 +1976,7 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="5">
+      <c r="A59">
         <v>10</v>
       </c>
       <c r="B59" t="s">
@@ -1992,7 +2002,7 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="5">
+      <c r="A60">
         <v>10</v>
       </c>
       <c r="B60" t="s">
@@ -2018,7 +2028,7 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="5">
+      <c r="A61">
         <v>10</v>
       </c>
       <c r="B61" t="s">
@@ -2044,7 +2054,7 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="5">
+      <c r="A62">
         <v>10</v>
       </c>
       <c r="B62" t="s">
@@ -2070,7 +2080,7 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="5">
+      <c r="A63">
         <v>10</v>
       </c>
       <c r="B63" t="s">
@@ -2096,7 +2106,7 @@
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="5">
+      <c r="A64">
         <v>10</v>
       </c>
       <c r="B64" t="s">
@@ -2122,7 +2132,7 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="5">
+      <c r="A65">
         <v>10</v>
       </c>
       <c r="B65" t="s">
@@ -2148,7 +2158,7 @@
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="5">
+      <c r="A66">
         <v>10</v>
       </c>
       <c r="B66" t="s">
@@ -2174,7 +2184,7 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="5">
+      <c r="A67">
         <v>10</v>
       </c>
       <c r="B67" t="s">
@@ -2200,7 +2210,7 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="5">
+      <c r="A68">
         <v>10</v>
       </c>
       <c r="B68" t="s">
@@ -2226,7 +2236,7 @@
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="5">
+      <c r="A69">
         <v>10</v>
       </c>
       <c r="B69" t="s">
@@ -2252,7 +2262,7 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="5">
+      <c r="A70">
         <v>10</v>
       </c>
       <c r="B70" t="s">
@@ -2278,7 +2288,7 @@
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="5">
+      <c r="A71">
         <v>10</v>
       </c>
       <c r="B71" t="s">
@@ -2304,7 +2314,7 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="5">
+      <c r="A72">
         <v>10</v>
       </c>
       <c r="B72" t="s">
@@ -2330,7 +2340,7 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="5">
+      <c r="A73">
         <v>10</v>
       </c>
       <c r="B73" t="s">
@@ -2356,7 +2366,7 @@
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="5">
+      <c r="A74">
         <v>10</v>
       </c>
       <c r="B74" t="s">
@@ -2382,7 +2392,7 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="5">
+      <c r="A75">
         <v>10</v>
       </c>
       <c r="B75" t="s">
@@ -2408,7 +2418,7 @@
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="5">
+      <c r="A76">
         <v>10</v>
       </c>
       <c r="B76" t="s">
@@ -2447,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2499,23 +2509,23 @@
         <f>main!B2</f>
         <v>Extra-trees</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <f>AVERAGE(main!C2:C6)</f>
         <v>88.894000000000005</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <f>AVERAGE(main!D2:D6)</f>
         <v>90.936000000000007</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <f>AVERAGE(main!E2:E6)</f>
         <v>46.75</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <f>AVERAGE(main!F2:F6)</f>
         <v>96.51</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <f>AVERAGE(main!G2:G6)</f>
         <v>11.106</v>
       </c>
@@ -2529,23 +2539,23 @@
         <f>main!B7</f>
         <v>SVM kernel linear</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <f>AVERAGE(main!C7:C11)</f>
         <v>88.246000000000009</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <f>AVERAGE(main!D7:D11)</f>
         <v>89.027999999999992</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <f>AVERAGE(main!E7:E11)</f>
         <v>33.08</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <f>AVERAGE(main!F7:F11)</f>
         <v>98.227999999999994</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <f>AVERAGE(main!G7:G11)</f>
         <v>11.754000000000001</v>
       </c>
@@ -2559,23 +2569,23 @@
         <f>main!B12</f>
         <v>SVM kernel poly</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <f>AVERAGE(main!C12:C16)</f>
         <v>87.921999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <f>AVERAGE(main!D12:D16)</f>
         <v>88.388000000000005</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <f>AVERAGE(main!E12:E16)</f>
         <v>28.297999999999995</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <f>AVERAGE(main!F12:F16)</f>
         <v>98.71</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <f>AVERAGE(main!G12:G16)</f>
         <v>12.077999999999999</v>
       </c>
@@ -2589,23 +2599,23 @@
         <f>main!B17</f>
         <v>SVM kernel rbf</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <f>AVERAGE(main!C17:C21)</f>
         <v>89.156000000000006</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <f>AVERAGE(main!D17:D21)</f>
         <v>90.070000000000007</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <f>AVERAGE(main!E17:E21)</f>
         <v>40.317999999999998</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <f>AVERAGE(main!F17:F21)</f>
         <v>98</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <f>AVERAGE(main!G17:G21)</f>
         <v>10.844000000000001</v>
       </c>
@@ -2619,23 +2629,23 @@
         <f>main!B22</f>
         <v>SVM kernel sigmoid</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <f>AVERAGE(main!C22:C26)</f>
         <v>73.299999999999983</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <f>AVERAGE(main!D22:D26)</f>
         <v>83.768000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>AVERAGE(main!E22:E26)</f>
         <v>8.9619999999999997</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <f>AVERAGE(main!F22:F26)</f>
         <v>84.93</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <f>AVERAGE(main!G22:G26)</f>
         <v>26.7</v>
       </c>
@@ -2649,23 +2659,23 @@
         <f>main!B27</f>
         <v>Extra-trees</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <f>AVERAGE(main!C27:C31)</f>
         <v>89.095999999999989</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <f>AVERAGE(main!D27:D31)</f>
         <v>91.003999999999991</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <f>AVERAGE(main!E27:E31)</f>
         <v>47.186</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <f>AVERAGE(main!F27:F31)</f>
         <v>96.691999999999993</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <f>AVERAGE(main!G27:G31)</f>
         <v>10.904</v>
       </c>
@@ -2679,23 +2689,23 @@
         <f>main!B32</f>
         <v>SVM kernel linear</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f>AVERAGE(main!C32:C36)</f>
         <v>88.254000000000005</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <f>AVERAGE(main!D32:D36)</f>
         <v>89.035999999999987</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <f>AVERAGE(main!E32:E36)</f>
         <v>33.070000000000007</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <f>AVERAGE(main!F32:F36)</f>
         <v>98.227999999999994</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <f>AVERAGE(main!G32:G36)</f>
         <v>11.746</v>
       </c>
@@ -2709,23 +2719,23 @@
         <f>main!B37</f>
         <v>SVM kernel poly</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <f>AVERAGE(main!C37:C41)</f>
         <v>87.947999999999993</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <f>AVERAGE(main!D37:D41)</f>
         <v>88.402000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <f>AVERAGE(main!E37:E41)</f>
         <v>28.378000000000004</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <f>AVERAGE(main!F37:F41)</f>
         <v>98.71599999999998</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <f>AVERAGE(main!G37:G41)</f>
         <v>12.052000000000001</v>
       </c>
@@ -2739,23 +2749,23 @@
         <f>main!B42</f>
         <v>SVM kernel rbf</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <f>AVERAGE(main!C42:C46)</f>
         <v>89.156000000000006</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <f>AVERAGE(main!D42:D46)</f>
         <v>90.1</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <f>AVERAGE(main!E42:E46)</f>
         <v>40.508000000000003</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <f>AVERAGE(main!F42:F46)</f>
         <v>97.953999999999994</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <f>AVERAGE(main!G42:G46)</f>
         <v>10.843999999999999</v>
       </c>
@@ -2769,23 +2779,23 @@
         <f>main!B47</f>
         <v>SVM kernel sigmoid</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <f>AVERAGE(main!C47:C51)</f>
         <v>73.202000000000012</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <f>AVERAGE(main!D47:D51)</f>
         <v>83.748000000000005</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <f>AVERAGE(main!E47:E51)</f>
         <v>8.8559999999999999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <f>AVERAGE(main!F47:F51)</f>
         <v>84.824000000000012</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <f>AVERAGE(main!G47:G51)</f>
         <v>26.798000000000002</v>
       </c>
@@ -2799,23 +2809,23 @@
         <f>main!B52</f>
         <v>Extra-trees</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <f>AVERAGE(main!C52:C56)</f>
         <v>89.122</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <f>AVERAGE(main!D52:D56)</f>
         <v>91.034000000000006</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <f>AVERAGE(main!E52:E56)</f>
         <v>47.464000000000006</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <f>AVERAGE(main!F52:F56)</f>
         <v>96.671999999999997</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <f>AVERAGE(main!G52:G56)</f>
         <v>10.878</v>
       </c>
@@ -2829,23 +2839,23 @@
         <f>main!B57</f>
         <v>SVM kernel linear</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <f>AVERAGE(main!C57:C61)</f>
         <v>88.23</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <f>AVERAGE(main!D57:D61)</f>
         <v>89.003999999999991</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <f>AVERAGE(main!E57:E61)</f>
         <v>32.828000000000003</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <f>AVERAGE(main!F57:F61)</f>
         <v>98.24799999999999</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <f>AVERAGE(main!G57:G61)</f>
         <v>11.77</v>
       </c>
@@ -2859,23 +2869,23 @@
         <f>main!B62</f>
         <v>SVM kernel poly</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <f>AVERAGE(main!C62:C66)</f>
         <v>87.921999999999997</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <f>AVERAGE(main!D62:D66)</f>
         <v>88.362000000000009</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <f>AVERAGE(main!E62:E66)</f>
         <v>28.060000000000002</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="4">
         <f>AVERAGE(main!F62:F66)</f>
         <v>98.744</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="4">
         <f>AVERAGE(main!G62:G66)</f>
         <v>12.077999999999999</v>
       </c>
@@ -2889,23 +2899,23 @@
         <f>main!B7</f>
         <v>SVM kernel linear</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <f>AVERAGE(main!C67:C71)</f>
         <v>89.126000000000005</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <f>AVERAGE(main!D67:D71)</f>
         <v>90.075999999999993</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <f>AVERAGE(main!E67:E71)</f>
         <v>40.436000000000007</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <f>AVERAGE(main!F67:F71)</f>
         <v>97.962000000000003</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="4">
         <f>AVERAGE(main!G67:G71)</f>
         <v>10.873999999999999</v>
       </c>
@@ -2919,23 +2929,23 @@
         <f>main!B72</f>
         <v>SVM kernel sigmoid</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <f>AVERAGE(main!C72:C76)</f>
         <v>73.25</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <f>AVERAGE(main!D72:D76)</f>
         <v>83.789999999999992</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <f>AVERAGE(main!E72:E76)</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <f>AVERAGE(main!F72:F76)</f>
         <v>84.808000000000007</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="4">
         <f>AVERAGE(main!G72:G76)</f>
         <v>26.75</v>
       </c>
@@ -2952,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B933AAEC-236B-4D22-AF27-850391C1FB4B}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3052,23 +3062,23 @@
         <f>main!H2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="7">
         <f>average!C2</f>
         <v>88.894000000000005</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="7">
         <f>average!D2</f>
         <v>90.936000000000007</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="7">
         <f>average!E2</f>
         <v>46.75</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="7">
         <f>average!F2</f>
         <v>96.51</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="7">
         <f>average!G2</f>
         <v>11.106</v>
       </c>
@@ -3106,11 +3116,11 @@
         <f>main!H3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
@@ -3145,11 +3155,11 @@
         <f>main!H4</f>
         <v>3</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
@@ -3184,11 +3194,11 @@
         <f>main!H5</f>
         <v>4</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
@@ -3223,11 +3233,11 @@
         <f>main!H6</f>
         <v>5</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
@@ -3262,23 +3272,23 @@
         <f>main!H7</f>
         <v>1</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="7">
         <f>average!C3</f>
         <v>88.246000000000009</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="7">
         <f>average!D3</f>
         <v>89.027999999999992</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="7">
         <f>average!E3</f>
         <v>33.08</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="7">
         <f>average!F3</f>
         <v>98.227999999999994</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="7">
         <f>average!G3</f>
         <v>11.754000000000001</v>
       </c>
@@ -3316,11 +3326,11 @@
         <f>main!H8</f>
         <v>2</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
@@ -3355,11 +3365,11 @@
         <f>main!H9</f>
         <v>3</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
@@ -3394,11 +3404,11 @@
         <f>main!H10</f>
         <v>4</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
@@ -3433,11 +3443,11 @@
         <f>main!H11</f>
         <v>5</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
@@ -3472,23 +3482,23 @@
         <f>main!H12</f>
         <v>1</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="7">
         <f>average!C4</f>
         <v>87.921999999999997</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="7">
         <f>average!D4</f>
         <v>88.388000000000005</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="7">
         <f>average!E4</f>
         <v>28.297999999999995</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="7">
         <f>average!F4</f>
         <v>98.71</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="7">
         <f>average!G4</f>
         <v>12.077999999999999</v>
       </c>
@@ -3526,11 +3536,11 @@
         <f>main!H13</f>
         <v>2</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
@@ -3565,11 +3575,11 @@
         <f>main!H14</f>
         <v>3</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
@@ -3604,11 +3614,11 @@
         <f>main!H15</f>
         <v>4</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
@@ -3643,11 +3653,11 @@
         <f>main!H16</f>
         <v>5</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
@@ -3682,23 +3692,23 @@
         <f>main!H17</f>
         <v>1</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="7">
         <f>average!C5</f>
         <v>89.156000000000006</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="7">
         <f>average!D5</f>
         <v>90.070000000000007</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="7">
         <f>average!E5</f>
         <v>40.317999999999998</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="7">
         <f>average!F5</f>
         <v>98</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="7">
         <f>average!G5</f>
         <v>10.844000000000001</v>
       </c>
@@ -3736,11 +3746,11 @@
         <f>main!H18</f>
         <v>2</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
@@ -3775,11 +3785,11 @@
         <f>main!H19</f>
         <v>3</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
@@ -3814,11 +3824,11 @@
         <f>main!H20</f>
         <v>4</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
@@ -3853,11 +3863,11 @@
         <f>main!H21</f>
         <v>5</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
@@ -3892,23 +3902,23 @@
         <f>main!H22</f>
         <v>1</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="7">
         <f>average!C6</f>
         <v>73.299999999999983</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="7">
         <f>average!D6</f>
         <v>83.768000000000001</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="7">
         <f>average!E6</f>
         <v>8.9619999999999997</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="7">
         <f>average!F6</f>
         <v>84.93</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="7">
         <f>average!G6</f>
         <v>26.7</v>
       </c>
@@ -3946,11 +3956,11 @@
         <f>main!H23</f>
         <v>2</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
@@ -3985,11 +3995,11 @@
         <f>main!H24</f>
         <v>3</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
@@ -4024,11 +4034,11 @@
         <f>main!H25</f>
         <v>4</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26">
@@ -4063,11 +4073,11 @@
         <f>main!H26</f>
         <v>5</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27">
@@ -4102,23 +4112,23 @@
         <f>main!H27</f>
         <v>1</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="7">
         <f>average!C7</f>
         <v>89.095999999999989</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="7">
         <f>average!D7</f>
         <v>91.003999999999991</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="7">
         <f>average!E7</f>
         <v>47.186</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="7">
         <f>average!F7</f>
         <v>96.691999999999993</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27" s="7">
         <f>average!G7</f>
         <v>10.904</v>
       </c>
@@ -4156,11 +4166,11 @@
         <f>main!H28</f>
         <v>2</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29">
@@ -4195,11 +4205,11 @@
         <f>main!H29</f>
         <v>3</v>
       </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30">
@@ -4234,11 +4244,11 @@
         <f>main!H30</f>
         <v>4</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31">
@@ -4273,11 +4283,11 @@
         <f>main!H31</f>
         <v>5</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32">
@@ -4312,23 +4322,23 @@
         <f>main!H32</f>
         <v>1</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="7">
         <f>average!C8</f>
         <v>88.254000000000005</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="7">
         <f>average!D8</f>
         <v>89.035999999999987</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="7">
         <f>average!E8</f>
         <v>33.070000000000007</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="7">
         <f>average!F8</f>
         <v>98.227999999999994</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="7">
         <f>average!G8</f>
         <v>11.746</v>
       </c>
@@ -4366,11 +4376,11 @@
         <f>main!H33</f>
         <v>2</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34">
@@ -4405,11 +4415,11 @@
         <f>main!H34</f>
         <v>3</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35">
@@ -4444,11 +4454,11 @@
         <f>main!H35</f>
         <v>4</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36">
@@ -4483,11 +4493,11 @@
         <f>main!H36</f>
         <v>5</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37">
@@ -4522,23 +4532,23 @@
         <f>main!H37</f>
         <v>1</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="7">
         <f>average!C9</f>
         <v>87.947999999999993</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="7">
         <f>average!D9</f>
         <v>88.402000000000001</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="7">
         <f>average!E9</f>
         <v>28.378000000000004</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="7">
         <f>average!F9</f>
         <v>98.71599999999998</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="7">
         <f>average!G9</f>
         <v>12.052000000000001</v>
       </c>
@@ -4576,11 +4586,11 @@
         <f>main!H38</f>
         <v>2</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39">
@@ -4615,11 +4625,11 @@
         <f>main!H39</f>
         <v>3</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40">
@@ -4654,11 +4664,11 @@
         <f>main!H40</f>
         <v>4</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41">
@@ -4693,11 +4703,11 @@
         <f>main!H41</f>
         <v>5</v>
       </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42">
@@ -4732,23 +4742,23 @@
         <f>main!H42</f>
         <v>1</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="7">
         <f>average!C10</f>
         <v>89.156000000000006</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="7">
         <f>average!D10</f>
         <v>90.1</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="7">
         <f>average!E10</f>
         <v>40.508000000000003</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="7">
         <f>average!F10</f>
         <v>97.953999999999994</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="7">
         <f>average!G10</f>
         <v>10.843999999999999</v>
       </c>
@@ -4786,11 +4796,11 @@
         <f>main!H43</f>
         <v>2</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44">
@@ -4825,11 +4835,11 @@
         <f>main!H44</f>
         <v>3</v>
       </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45">
@@ -4864,11 +4874,11 @@
         <f>main!H45</f>
         <v>4</v>
       </c>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46">
@@ -4903,11 +4913,11 @@
         <f>main!H46</f>
         <v>5</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47">
@@ -4942,23 +4952,23 @@
         <f>main!H47</f>
         <v>1</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47" s="7">
         <f>average!C11</f>
         <v>73.202000000000012</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="7">
         <f>average!D11</f>
         <v>83.748000000000005</v>
       </c>
-      <c r="K47" s="4">
+      <c r="K47" s="7">
         <f>average!E11</f>
         <v>8.8559999999999999</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47" s="7">
         <f>average!F11</f>
         <v>84.824000000000012</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47" s="7">
         <f>average!G11</f>
         <v>26.798000000000002</v>
       </c>
@@ -4996,11 +5006,11 @@
         <f>main!H48</f>
         <v>2</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49">
@@ -5035,11 +5045,11 @@
         <f>main!H49</f>
         <v>3</v>
       </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50">
@@ -5074,11 +5084,11 @@
         <f>main!H50</f>
         <v>4</v>
       </c>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51">
@@ -5113,11 +5123,11 @@
         <f>main!H51</f>
         <v>5</v>
       </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52">
@@ -5152,23 +5162,23 @@
         <f>main!H52</f>
         <v>1</v>
       </c>
-      <c r="I52" s="4">
+      <c r="I52" s="7">
         <f>average!C12</f>
         <v>89.122</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="7">
         <f>average!D12</f>
         <v>91.034000000000006</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="7">
         <f>average!E12</f>
         <v>47.464000000000006</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="7">
         <f>average!F12</f>
         <v>96.671999999999997</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52" s="7">
         <f>average!G12</f>
         <v>10.878</v>
       </c>
@@ -5206,11 +5216,11 @@
         <f>main!H53</f>
         <v>2</v>
       </c>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54">
@@ -5245,11 +5255,11 @@
         <f>main!H54</f>
         <v>3</v>
       </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55">
@@ -5284,11 +5294,11 @@
         <f>main!H55</f>
         <v>4</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56">
@@ -5323,11 +5333,11 @@
         <f>main!H56</f>
         <v>5</v>
       </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57">
@@ -5362,23 +5372,23 @@
         <f>main!H57</f>
         <v>1</v>
       </c>
-      <c r="I57" s="4">
+      <c r="I57" s="7">
         <f>average!C13</f>
         <v>88.23</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="7">
         <f>average!D13</f>
         <v>89.003999999999991</v>
       </c>
-      <c r="K57" s="4">
+      <c r="K57" s="7">
         <f>average!E13</f>
         <v>32.828000000000003</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L57" s="7">
         <f>average!F13</f>
         <v>98.24799999999999</v>
       </c>
-      <c r="M57" s="4">
+      <c r="M57" s="7">
         <f>average!G13</f>
         <v>11.77</v>
       </c>
@@ -5416,11 +5426,11 @@
         <f>main!H58</f>
         <v>2</v>
       </c>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59">
@@ -5455,11 +5465,11 @@
         <f>main!H59</f>
         <v>3</v>
       </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60">
@@ -5494,11 +5504,11 @@
         <f>main!H60</f>
         <v>4</v>
       </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61">
@@ -5533,11 +5543,11 @@
         <f>main!H61</f>
         <v>5</v>
       </c>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
     </row>
     <row r="62" spans="1:13">
       <c r="A62">
@@ -5572,23 +5582,23 @@
         <f>main!H62</f>
         <v>1</v>
       </c>
-      <c r="I62" s="4">
+      <c r="I62" s="7">
         <f>average!C14</f>
         <v>87.921999999999997</v>
       </c>
-      <c r="J62" s="4">
+      <c r="J62" s="7">
         <f>average!D14</f>
         <v>88.362000000000009</v>
       </c>
-      <c r="K62" s="4">
+      <c r="K62" s="7">
         <f>average!E14</f>
         <v>28.060000000000002</v>
       </c>
-      <c r="L62" s="4">
+      <c r="L62" s="7">
         <f>average!F14</f>
         <v>98.744</v>
       </c>
-      <c r="M62" s="4">
+      <c r="M62" s="7">
         <f>average!G14</f>
         <v>12.077999999999999</v>
       </c>
@@ -5626,11 +5636,11 @@
         <f>main!H63</f>
         <v>2</v>
       </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64">
@@ -5665,11 +5675,11 @@
         <f>main!H64</f>
         <v>3</v>
       </c>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65">
@@ -5704,11 +5714,11 @@
         <f>main!H65</f>
         <v>4</v>
       </c>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66">
@@ -5743,11 +5753,11 @@
         <f>main!H66</f>
         <v>5</v>
       </c>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67">
@@ -5782,23 +5792,23 @@
         <f>main!H67</f>
         <v>1</v>
       </c>
-      <c r="I67" s="4">
+      <c r="I67" s="7">
         <f>average!C15</f>
         <v>89.126000000000005</v>
       </c>
-      <c r="J67" s="4">
+      <c r="J67" s="7">
         <f>average!D15</f>
         <v>90.075999999999993</v>
       </c>
-      <c r="K67" s="4">
+      <c r="K67" s="7">
         <f>average!E15</f>
         <v>40.436000000000007</v>
       </c>
-      <c r="L67" s="4">
+      <c r="L67" s="7">
         <f>average!F15</f>
         <v>97.962000000000003</v>
       </c>
-      <c r="M67" s="4">
+      <c r="M67" s="7">
         <f>average!G15</f>
         <v>10.873999999999999</v>
       </c>
@@ -5836,11 +5846,11 @@
         <f>main!H68</f>
         <v>2</v>
       </c>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69">
@@ -5875,11 +5885,11 @@
         <f>main!H69</f>
         <v>3</v>
       </c>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70">
@@ -5914,11 +5924,11 @@
         <f>main!H70</f>
         <v>4</v>
       </c>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71">
@@ -5953,11 +5963,11 @@
         <f>main!H71</f>
         <v>5</v>
       </c>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72">
@@ -5992,23 +6002,23 @@
         <f>main!H72</f>
         <v>1</v>
       </c>
-      <c r="I72" s="4">
+      <c r="I72" s="7">
         <f>average!C16</f>
         <v>73.25</v>
       </c>
-      <c r="J72" s="4">
+      <c r="J72" s="7">
         <f>average!D16</f>
         <v>83.789999999999992</v>
       </c>
-      <c r="K72" s="4">
+      <c r="K72" s="7">
         <f>average!E16</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="L72" s="4">
+      <c r="L72" s="7">
         <f>average!F16</f>
         <v>84.808000000000007</v>
       </c>
-      <c r="M72" s="4">
+      <c r="M72" s="7">
         <f>average!G16</f>
         <v>26.75</v>
       </c>
@@ -6046,11 +6056,11 @@
         <f>main!H73</f>
         <v>2</v>
       </c>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74">
@@ -6085,11 +6095,11 @@
         <f>main!H74</f>
         <v>3</v>
       </c>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75">
@@ -6124,11 +6134,11 @@
         <f>main!H75</f>
         <v>4</v>
       </c>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
     </row>
     <row r="76" spans="1:13">
       <c r="A76">
@@ -6163,11 +6173,11 @@
         <f>main!H76</f>
         <v>5</v>
       </c>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="75">

</xml_diff>